<commit_message>
backpressure, CICD_kinds, money_korean, excel, fs_folder, JSDoc, Todo: .bashrc
</commit_message>
<xml_diff>
--- a/Language/Javascript/node/modules/excel/target/specification_org.xlsx
+++ b/Language/Javascript/node/modules/excel/target/specification_org.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\20151224\유전자분양\서류_견본\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\line\Desktop\git_folder\pmp\Language\Javascript\node\modules\excel\target\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -690,6 +690,60 @@
     <xf numFmtId="41" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -727,60 +781,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="17" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="14" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1154,7 +1154,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1"/>
@@ -1173,17 +1173,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="47.25" customHeight="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1">
@@ -1211,7 +1211,7 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="71" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="36" t="s">
@@ -1221,20 +1221,20 @@
         <v>13</v>
       </c>
       <c r="D4" s="25"/>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="73" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
     </row>
     <row r="5" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A5" s="54"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="36" t="s">
         <v>31</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>34</v>
       </c>
       <c r="D5" s="29"/>
-      <c r="E5" s="55"/>
+      <c r="E5" s="73"/>
       <c r="F5" s="40" t="s">
         <v>24</v>
       </c>
@@ -1258,7 +1258,7 @@
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A6" s="54"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="36" t="s">
         <v>7</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="30"/>
-      <c r="E6" s="55"/>
+      <c r="E6" s="73"/>
       <c r="F6" s="41" t="s">
         <v>25</v>
       </c>
@@ -1278,7 +1278,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A7" s="54"/>
+      <c r="A7" s="72"/>
       <c r="B7" s="36" t="s">
         <v>32</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="30"/>
-      <c r="E7" s="55"/>
+      <c r="E7" s="73"/>
       <c r="F7" s="41" t="s">
         <v>26</v>
       </c>
@@ -1301,13 +1301,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A8" s="54"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="36" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="30"/>
-      <c r="E8" s="55"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="41" t="s">
         <v>37</v>
       </c>
@@ -1336,9 +1336,9 @@
       <c r="A10" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
       <c r="E10" s="33"/>
       <c r="F10" s="23"/>
       <c r="G10" s="27"/>
@@ -1347,26 +1347,26 @@
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" s="11" customFormat="1" ht="24" customHeight="1">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="48"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="66"/>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="18" t="s">
         <v>3</v>
       </c>
@@ -1376,19 +1376,19 @@
       <c r="G12" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="51" t="s">
+      <c r="H12" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="52"/>
+      <c r="I12" s="70"/>
       <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="60"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="47"/>
       <c r="E13" s="15">
         <v>70000</v>
       </c>
@@ -1399,245 +1399,251 @@
         <f t="shared" ref="G13" si="0">E13*F13</f>
         <v>70000</v>
       </c>
-      <c r="H13" s="61">
+      <c r="H13" s="48">
         <f t="shared" ref="H13" si="1">E13/10</f>
         <v>7000</v>
       </c>
-      <c r="I13" s="62"/>
+      <c r="I13" s="49"/>
       <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A14" s="63" t="s">
+      <c r="A14" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="65"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="15"/>
       <c r="F14" s="16"/>
       <c r="G14" s="21"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="62"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="49"/>
       <c r="J14" s="13"/>
     </row>
     <row r="15" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A15" s="63"/>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="65"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="15"/>
       <c r="F15" s="20"/>
       <c r="G15" s="21"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="62"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="49"/>
       <c r="J15" s="13"/>
     </row>
     <row r="16" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A16" s="63"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="65"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="15"/>
       <c r="F16" s="20"/>
       <c r="G16" s="21"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="62"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="49"/>
       <c r="J16" s="13"/>
     </row>
     <row r="17" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A17" s="63"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="65"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="15"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="62"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="13"/>
     </row>
     <row r="18" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A18" s="63"/>
-      <c r="B18" s="64"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="65"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="15"/>
       <c r="F18" s="20"/>
       <c r="G18" s="21"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="62"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="49"/>
       <c r="J18" s="13"/>
     </row>
     <row r="19" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A19" s="63"/>
-      <c r="B19" s="64"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="65"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
       <c r="E19" s="15"/>
       <c r="F19" s="20"/>
       <c r="G19" s="21"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="62"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="49"/>
       <c r="J19" s="13"/>
     </row>
     <row r="20" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A20" s="63"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="65"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
       <c r="E20" s="15"/>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="62"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="49"/>
       <c r="J20" s="13"/>
     </row>
     <row r="21" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A21" s="58"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="60"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="47"/>
       <c r="E21" s="15"/>
       <c r="F21" s="20"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="62"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="49"/>
       <c r="J21" s="13"/>
     </row>
     <row r="22" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A22" s="63"/>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="65"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="15"/>
       <c r="F22" s="20"/>
       <c r="G22" s="21"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="62"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="49"/>
       <c r="J22" s="13"/>
     </row>
     <row r="23" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A23" s="63"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="65"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="52"/>
       <c r="E23" s="15"/>
       <c r="F23" s="20"/>
       <c r="G23" s="21"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="62"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="49"/>
       <c r="J23" s="13"/>
     </row>
     <row r="24" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A24" s="58"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="60"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="47"/>
       <c r="E24" s="15"/>
       <c r="F24" s="20"/>
       <c r="G24" s="21"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="62"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="49"/>
       <c r="J24" s="13"/>
     </row>
     <row r="25" spans="1:10" s="14" customFormat="1" ht="24" customHeight="1">
-      <c r="A25" s="58"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="60"/>
+      <c r="A25" s="45"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="47"/>
       <c r="E25" s="15"/>
       <c r="F25" s="20"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="62"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="49"/>
       <c r="J25" s="13"/>
     </row>
     <row r="26" spans="1:10" s="8" customFormat="1" ht="24" customHeight="1">
-      <c r="A26" s="58"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="60"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="47"/>
       <c r="E26" s="15"/>
       <c r="F26" s="20"/>
       <c r="G26" s="21"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="62"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="49"/>
       <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:10" s="8" customFormat="1" ht="24" customHeight="1">
-      <c r="A27" s="63"/>
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="65"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="52"/>
       <c r="E27" s="15"/>
       <c r="F27" s="20"/>
       <c r="G27" s="21"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="75"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="54"/>
       <c r="J27" s="17"/>
     </row>
     <row r="28" spans="1:10" ht="24" customHeight="1">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="68">
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="57">
         <f>SUM(G13:G27)</f>
         <v>70000</v>
       </c>
-      <c r="H28" s="68"/>
-      <c r="I28" s="69"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="58"/>
     </row>
     <row r="29" spans="1:10" ht="24" customHeight="1">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="68">
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="57">
         <f>SUM(H13:I27)</f>
         <v>7000</v>
       </c>
-      <c r="H29" s="68"/>
-      <c r="I29" s="69"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="58"/>
     </row>
     <row r="30" spans="1:10" ht="24" customHeight="1" thickBot="1">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="72">
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="61">
         <f>SUM(G28:I29)</f>
         <v>77000</v>
       </c>
-      <c r="H30" s="72"/>
-      <c r="I30" s="73"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="E4:E8"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="H23:I23"/>
@@ -1652,24 +1658,18 @@
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="A23:D23"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="E4:E8"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="H27:I27"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>